<commit_message>
Remove the redundancy of the code
</commit_message>
<xml_diff>
--- a/SpecificPricing_TestData.xlsx
+++ b/SpecificPricing_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RateCard &amp; Pricing" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -248,7 +248,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -318,10 +318,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -329,15 +329,13 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.8962962962963"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.3666666666667"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.2296296296296"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.5444444444444"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.2592592592593"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.5222222222222"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.9111111111111"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="3.52962962962963"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="5.97777777777778"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="6.27037037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="1020" min="9" style="1" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="1021" style="0" width="14.3074074074074"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -366,19 +364,18 @@
         <v>15</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -402,7 +399,7 @@
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Modify the Code for the Mediation Configuration
</commit_message>
<xml_diff>
--- a/SpecificPricing_TestData.xlsx
+++ b/SpecificPricing_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="RateCard &amp; Pricing" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -98,13 +98,13 @@
     <t xml:space="preserve">Test Mediation</t>
   </si>
   <si>
+    <t xml:space="preserve">com.sapienter.jbilling.server.mediation.task.SeparatorFileReader</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asterisk</t>
+  </si>
+  <si>
     <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.sapienter.jbilling.server.mediation.task.SeparatorFileReader</t>
-  </si>
-  <si>
-    <t xml:space="preserve">asterisk</t>
   </si>
   <si>
     <t xml:space="preserve">csv</t>
@@ -247,19 +247,19 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="K1 E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.4259259259259"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="15.2888888888889"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="15.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -305,7 +305,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -320,22 +320,22 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1" activeCellId="1" sqref="K1 I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.8962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.3666666666667"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.2592592592593"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="3.52962962962963"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="5.97777777777778"/>
-    <col collapsed="false" hidden="false" max="1020" min="9" style="1" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="1021" style="0" width="14.3074074074074"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="3.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="5.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="9" style="1" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1021" style="0" width="14.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -384,7 +384,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -399,25 +399,25 @@
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="K1 D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.8555555555556"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.8333333333333"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="31.062962962963"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="31.5555555555556"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="23.5185185185185"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="27.6333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="14.3074074074074"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="31.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="20.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="31.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="23.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="21.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="27.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="1" width="14.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -461,7 +461,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -474,30 +474,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M7" activeCellId="0" sqref="M7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.0740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.62222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.937037037037"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.62222222222222"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="34.2925925925926"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.62222222222222"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="4.32962962962963"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.62222222222222"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="18.4555555555556"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="5.03703703703704"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="46.0888888888889"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="8.62222222222222"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="34.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="4.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="8.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="5.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="46.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="15.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="13" style="1" width="8.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="8.36"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,22 +521,22 @@
         <v>26</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -544,7 +545,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -559,20 +560,20 @@
   </sheetPr>
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I3" activeCellId="1" sqref="K1 I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="8.62222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.5444444444444"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.1074074074074"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="8.62222222222222"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.3259259259259"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.7407407407407"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="8.62222222222222"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="8.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="8.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="1" width="8.62"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -623,7 +624,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Completed the Test Plan Only asserts are left to add
</commit_message>
<xml_diff>
--- a/SpecificPricing_TestData.xlsx
+++ b/SpecificPricing_TestData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -123,6 +123,12 @@
   </si>
   <si>
     <t xml:space="preserve">pre paid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$37,650.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$4900</t>
   </si>
 </sst>
 </file>
@@ -133,7 +139,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -164,6 +170,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -207,7 +219,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -228,6 +240,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -248,7 +264,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="K1 E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="F:F E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -321,19 +337,19 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="1" sqref="K1 I1"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="1" sqref="F:F I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="3.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="5.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="5.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="9" style="1" width="14.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1021" style="0" width="14.31"/>
   </cols>
@@ -400,7 +416,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="K1 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="F:F D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -477,7 +493,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F:F"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -486,7 +502,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="34.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="71.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="4.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="8.62"/>
@@ -558,10 +574,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="1" sqref="K1 I3"/>
+      <selection pane="topLeft" activeCell="K8" activeCellId="1" sqref="F:F K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -573,10 +589,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="1" width="8.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="8.62"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -604,6 +621,10 @@
       <c r="I1" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="J1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="1" t="s">
@@ -611,6 +632,9 @@
       </c>
       <c r="G2" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Add Assert in SpecificPricingPage
</commit_message>
<xml_diff>
--- a/SpecificPricing_TestData.xlsx
+++ b/SpecificPricing_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="RateCard &amp; Pricing" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="57">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -98,15 +98,15 @@
     <t xml:space="preserve">Test Mediation</t>
   </si>
   <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
     <t xml:space="preserve">com.sapienter.jbilling.server.mediation.task.SeparatorFileReader</t>
   </si>
   <si>
     <t xml:space="preserve">asterisk</t>
   </si>
   <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
     <t xml:space="preserve">csv</t>
   </si>
   <si>
@@ -125,10 +125,76 @@
     <t xml:space="preserve">pre paid</t>
   </si>
   <si>
+    <t xml:space="preserve">US$4,950.00</t>
+  </si>
+  <si>
     <t xml:space="preserve">US$37,650.00</t>
   </si>
   <si>
-    <t xml:space="preserve">US$4900</t>
+    <t xml:space="preserve">300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$0.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$150.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$1.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$600.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$15.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$6,000.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$2.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$1,250.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$5.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$2,500.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$3.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$700.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$20.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$4,000.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$4.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$2,250.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$50.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$25,000.00</t>
   </si>
 </sst>
 </file>
@@ -139,7 +205,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -170,12 +236,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -219,7 +279,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -238,10 +298,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -263,19 +319,19 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="F:F E1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="Q12:Q18 E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="15.29"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="15.2888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -321,7 +377,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -336,22 +392,22 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="1" sqref="F:F I1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="1" sqref="Q12:Q18 G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="3.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="5.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="9" style="1" width="14.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1021" style="0" width="14.31"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.8962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.3666666666667"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.2592592592593"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="3.52962962962963"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="5.97777777777778"/>
+    <col collapsed="false" hidden="false" max="1020" min="9" style="1" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="1021" style="0" width="14.3074074074074"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -400,7 +456,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -415,25 +471,25 @@
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="F:F D2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="Q12:Q18 D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="31.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="20.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="31.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="23.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="21.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="27.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="1" width="14.31"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.8555555555556"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.8333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="31.062962962963"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="31.5555555555556"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="23.5185185185185"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="27.6333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="14.3074074074074"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -477,7 +533,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -490,31 +546,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F:F"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M7" activeCellId="1" sqref="Q12:Q18 M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="71.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="4.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="8.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="5.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="46.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="15.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="13" style="1" width="8.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="8.36"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.937037037037"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="34.2925925925926"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="4.32962962962963"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="18.4555555555556"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="5.03703703703704"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="46.0888888888889"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="8.62222222222222"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -537,22 +592,22 @@
         <v>26</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="L1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E2" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -561,7 +616,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -574,26 +629,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K8" activeCellId="1" sqref="F:F K8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q12" activeCellId="0" sqref="Q12:Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="8.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="8.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="8.62"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.5444444444444"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.1074074074074"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.3259259259259"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.7407407407407"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="14.9259259259259"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="1" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="13.6148148148148"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="14.1185185185185"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="1" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="13.5111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="1" width="8.62222222222222"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -624,31 +684,142 @@
       <c r="J1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+    </row>
+    <row r="2" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="1" t="s">
         <v>21</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D3" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
+      <c r="K3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" display="WebData@123"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Added Validation for the Product and Customer Controller
</commit_message>
<xml_diff>
--- a/SpecificPricing_TestData.xlsx
+++ b/SpecificPricing_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="RateCard &amp; Pricing" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="59">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -53,10 +53,16 @@
     <t xml:space="preserve">dst</t>
   </si>
   <si>
+    <t xml:space="preserve">rate_test_ratecard</t>
+  </si>
+  <si>
     <t xml:space="preserve">Plan RateCard</t>
   </si>
   <si>
     <t xml:space="preserve">Plan Pricing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rate_plan_ratecard</t>
   </si>
   <si>
     <t xml:space="preserve">Test Category</t>
@@ -292,12 +298,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -317,24 +323,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="Q12:Q18 E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.4259259259259"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="15.2888888888889"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="1" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="15.29"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -362,13 +370,19 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -377,7 +391,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -392,62 +406,62 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="1" sqref="Q12:Q18 G2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.8962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.3666666666667"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.2592592592593"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="3.52962962962963"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="5.97777777777778"/>
-    <col collapsed="false" hidden="false" max="1020" min="9" style="1" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="1021" style="0" width="14.3074074074074"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="3.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="5.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="9" style="1" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1021" style="0" width="14.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -456,7 +470,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -471,59 +485,59 @@
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="Q12:Q18 D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.8555555555556"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.8333333333333"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="31.062962962963"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="31.5555555555556"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="23.5185185185185"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="27.6333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="14.3074074074074"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="31.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="20.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="31.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="23.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="21.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="27.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="1" width="14.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="19.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -533,7 +547,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -548,66 +562,66 @@
   </sheetPr>
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M7" activeCellId="1" sqref="Q12:Q18 M7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M7" activeCellId="0" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.0740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.62222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.937037037037"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.62222222222222"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="34.2925925925926"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.62222222222222"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="4.32962962962963"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.62222222222222"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="18.4555555555556"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="5.03703703703704"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="46.0888888888889"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="8.62222222222222"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="34.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="4.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="8.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="18.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="5.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="46.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="1" width="8.62"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -616,7 +630,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -631,176 +645,176 @@
   </sheetPr>
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q12" activeCellId="0" sqref="Q12:Q18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q12" activeCellId="0" sqref="Q12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="8.62222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.5444444444444"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.1074074074074"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="8.62222222222222"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.3259259259259"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.7407407407407"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="14.9259259259259"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="1" width="8.62222222222222"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="13.6148148148148"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="14.1185185185185"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="1" width="8.62222222222222"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="13.5111111111111"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="1" width="8.62222222222222"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="8.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="8.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="8.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="13.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="14.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="1" width="8.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="1" width="8.62"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
+        <v>25</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="M2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="O2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q2" s="4" t="s">
+      <c r="L2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>37</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="M3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="O3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="P3" s="4" t="s">
+      <c r="L3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="M3" s="3" t="s">
         <v>42</v>
       </c>
+      <c r="O3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="M4" s="4" t="s">
+      <c r="K4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="O4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="P4" s="4" t="s">
+      <c r="L4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="M4" s="3" t="s">
         <v>47</v>
       </c>
+      <c r="O4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K5" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="M5" s="4" t="s">
+      <c r="K5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="O5" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="P5" s="4" t="s">
+      <c r="L5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="M5" s="3" t="s">
         <v>52</v>
       </c>
+      <c r="O5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K6" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="P6" s="4" t="s">
+      <c r="K6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="Q6" s="4" t="s">
+      <c r="M6" s="3" t="s">
         <v>56</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -819,7 +833,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Added Validation for MediationConfigurationTest
</commit_message>
<xml_diff>
--- a/SpecificPricing_TestData.xlsx
+++ b/SpecificPricing_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="RateCard &amp; Pricing" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="60">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -53,16 +53,13 @@
     <t xml:space="preserve">dst</t>
   </si>
   <si>
-    <t xml:space="preserve">rate_test_ratecard</t>
-  </si>
-  <si>
     <t xml:space="preserve">Plan RateCard</t>
   </si>
   <si>
     <t xml:space="preserve">Plan Pricing</t>
   </si>
   <si>
-    <t xml:space="preserve">rate_plan_ratecard</t>
+    <t xml:space="preserve">Web Data 11</t>
   </si>
   <si>
     <t xml:space="preserve">Test Category</t>
@@ -77,16 +74,22 @@
     <t xml:space="preserve">10</t>
   </si>
   <si>
+    <t xml:space="preserve">Items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMPONENT PRICES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Pricing Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Pricing Product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20</t>
+  </si>
+  <si>
     <t xml:space="preserve">Plan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plan Pricing Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plan Pricing Product</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20</t>
   </si>
   <si>
     <t xml:space="preserve">Default</t>
@@ -298,12 +301,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -323,26 +326,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="1" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="15.29"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.0148148148148"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="16.0703703703704"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -370,19 +371,13 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -391,7 +386,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -404,53 +399,57 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="3.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="5.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="9" style="1" width="14.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1021" style="0" width="14.31"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.2888888888889"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.1481481481481"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.262962962963"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="3.52962962962963"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="6.17407407407407"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.3518518518519"/>
+    <col collapsed="false" hidden="false" max="1020" min="11" style="1" width="14.8962962962963"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -462,6 +461,9 @@
       </c>
       <c r="G2" s="1" t="s">
         <v>20</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -470,7 +472,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -485,59 +487,60 @@
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="31.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="20.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="31.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="23.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="21.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="27.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="1" width="14.31"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.3481481481481"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.8111111111111"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="32.5333333333333"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="33.1222222222222"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="24.6962962962963"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="28.9074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="14.8962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="19.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E2" s="1" t="s">
-        <v>23</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="F2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E3" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -547,7 +550,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -560,68 +563,70 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M7" activeCellId="0" sqref="M7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="34.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="4.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="8.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="18.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="5.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="46.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="1" width="8.62"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.662962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.5222222222222"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="84.0185185185185"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="4.50740740740741"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="5.19259259259259"/>
+    <col collapsed="false" hidden="false" max="1023" min="12" style="1" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F2" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -630,7 +635,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -645,176 +650,176 @@
   </sheetPr>
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="Q12" activeCellId="0" sqref="Q12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="8.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="8.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="8.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="13.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="14.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="1" width="8.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="1" width="8.62"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.937037037037"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.9925925925926"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.1074074074074"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.2296296296296"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="1" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="14.2074074074074"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="14.7"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="1" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="14.1111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="1" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" s="3" t="s">
+      <c r="K2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="L2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="P2" s="3" t="s">
+      <c r="M2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="P2" s="4" t="s">
         <v>39</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="L3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="L3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="O3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="P3" s="3" t="s">
+      <c r="M3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="O3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="P3" s="4" t="s">
         <v>44</v>
       </c>
+      <c r="Q3" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L4" s="3" t="s">
+      <c r="K4" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="L4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="O4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="P4" s="3" t="s">
+      <c r="M4" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="O4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="P4" s="4" t="s">
         <v>49</v>
       </c>
+      <c r="Q4" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K5" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="L5" s="3" t="s">
+      <c r="K5" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="L5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="O5" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="P5" s="3" t="s">
+      <c r="M5" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="Q5" s="3" t="s">
+      <c r="O5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="P5" s="4" t="s">
         <v>54</v>
       </c>
+      <c r="Q5" s="4" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="M6" s="3" t="s">
+      <c r="K6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="O6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="P6" s="3" t="s">
+      <c r="M6" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="Q6" s="3" t="s">
+      <c r="O6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="P6" s="4" t="s">
         <v>58</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -833,7 +838,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Added a column for the rate card csv name
</commit_message>
<xml_diff>
--- a/SpecificPricing_TestData.xlsx
+++ b/SpecificPricing_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="RateCard &amp; Pricing" sheetId="1" state="visible" r:id="rId2"/>
@@ -328,19 +328,19 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="16.0703703703704"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="16.07"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -386,7 +386,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -401,23 +401,24 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.2888888888889"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.1481481481481"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="3.52962962962963"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="6.17407407407407"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.3518518518519"/>
-    <col collapsed="false" hidden="false" max="1020" min="11" style="1" width="14.8962962962963"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="3.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="6.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="11" style="1" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1021" style="0" width="8.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -472,7 +473,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -487,25 +488,25 @@
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.3481481481481"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.8111111111111"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="32.5333333333333"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="33.1222222222222"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="24.6962962962963"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="28.9074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="14.8962962962963"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="32.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="21.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="33.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="24.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="22.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="28.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="1" width="14.9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -550,7 +551,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -565,25 +566,25 @@
   </sheetPr>
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.662962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.5222222222222"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="84.0185185185185"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="4.50740740740741"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="5.19259259259259"/>
-    <col collapsed="false" hidden="false" max="1023" min="12" style="1" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.01481481481481"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="84.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="4.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="19.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="5.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="12" style="1" width="9.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.01"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -635,7 +636,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -650,26 +651,26 @@
   </sheetPr>
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="Q12" activeCellId="0" sqref="Q12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.937037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.9925925925926"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.1074074074074"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.2296296296296"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="1" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="14.2074074074074"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="14.7"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="1" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="14.1111111111111"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="1" width="9.01481481481481"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="9.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="9.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="9.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="1" width="9.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="1" width="9.01"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -838,7 +839,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Specific Pricing Testing and done the changes
</commit_message>
<xml_diff>
--- a/SpecificPricing_TestData.xlsx
+++ b/SpecificPricing_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="RateCard &amp; Pricing" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="64">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -32,7 +32,7 @@
     <t xml:space="preserve">WebData@123</t>
   </si>
   <si>
-    <t xml:space="preserve">Web Data 18</t>
+    <t xml:space="preserve">Web Data 26</t>
   </si>
   <si>
     <t xml:space="preserve">Test RateCard</t>
@@ -53,13 +53,22 @@
     <t xml:space="preserve">dst</t>
   </si>
   <si>
+    <t xml:space="preserve">rate_test_ratecard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/test_rate_card.csv</t>
+  </si>
+  <si>
     <t xml:space="preserve">Plan RateCard</t>
   </si>
   <si>
     <t xml:space="preserve">Plan Pricing</t>
   </si>
   <si>
-    <t xml:space="preserve">Web Data 11</t>
+    <t xml:space="preserve">rate_plan_ratecard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/plan_rate_card.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Test Category</t>
@@ -77,9 +86,6 @@
     <t xml:space="preserve">Items</t>
   </si>
   <si>
-    <t xml:space="preserve">COMPONENT PRICES</t>
-  </si>
-  <si>
     <t xml:space="preserve">Plan Pricing Category</t>
   </si>
   <si>
@@ -140,6 +146,9 @@
     <t xml:space="preserve">US$37,650.00</t>
   </si>
   <si>
+    <t xml:space="preserve">/MediationPlanPricing.csv</t>
+  </si>
+  <si>
     <t xml:space="preserve">300</t>
   </si>
   <si>
@@ -147,6 +156,9 @@
   </si>
   <si>
     <t xml:space="preserve">US$150.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/MediationTestPricing.csv</t>
   </si>
   <si>
     <t xml:space="preserve">400</t>
@@ -301,12 +313,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -326,10 +338,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -343,7 +355,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="16.07"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -371,13 +383,25 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -399,10 +423,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="1" sqref="C1 J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -415,56 +439,52 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="3.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="6.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="11" style="1" width="14.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1021" style="0" width="8.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1019" min="9" style="1" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1020" style="0" width="8.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="8.36"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -489,12 +509,12 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="1" sqref="C1 F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.46"/>
@@ -502,7 +522,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="32.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="21.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="33.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="33.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="24.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="22.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="28.91"/>
@@ -513,35 +533,35 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="19.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="E2" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E3" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -564,10 +584,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="1" sqref="C1 H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -575,59 +595,55 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="84.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="4.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="19.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="5.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="12" style="1" width="9.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="9.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="19.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="5.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="11" style="1" width="9.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1023" style="0" width="9.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="8.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F2" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -649,10 +665,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q12" activeCellId="0" sqref="Q12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -670,157 +686,164 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="14.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="1" width="9.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="1" width="9.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="22.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="1" width="9.01"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D2" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>40</v>
+        <v>21</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>45</v>
       </c>
+      <c r="L3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K4" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q4" s="4" t="s">
+      <c r="K4" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="L4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q5" s="4" t="s">
+      <c r="K5" s="3" t="s">
         <v>55</v>
       </c>
+      <c r="L5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K6" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q6" s="4" t="s">
-        <v>59</v>
+      <c r="K6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
bugfixes for the Specific Pricing Feature
</commit_message>
<xml_diff>
--- a/SpecificPricing_TestData.xlsx
+++ b/SpecificPricing_TestData.xlsx
@@ -15,207 +15,202 @@
     <sheet name="Orders" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="64">
   <si>
-    <t xml:space="preserve">admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WebData@123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Web Data 26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test RateCard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Pricing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RATE_CARD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">match_column</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dst</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rate_test_ratecard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/test_rate_card.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plan RateCard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plan Pricing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rate_plan_ratecard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/plan_rate_card.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Product</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United States Dollar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Items</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plan Pricing Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plan Pricing Product</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Customer1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Customer2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Customer3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test Mediation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.sapienter.jbilling.server.mediation.task.SeparatorFileReader</t>
-  </si>
-  <si>
-    <t xml:space="preserve">asterisk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">yyyyMMdd-HHmmss</t>
-  </si>
-  <si>
-    <t xml:space="preserve">,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">in.webdataconsulting.jbilling.server.mediation.tasks.WebDataTestAsteriskMediationTask</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Monthly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pre paid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US$4,950.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US$37,650.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/MediationPlanPricing.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US$0.50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US$150.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/MediationTestPricing.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">400</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US$1.50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US$600.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US$15.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US$6,000.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US$2.50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US$1,250.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US$5.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US$2,500.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">200</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US$3.50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US$700.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US$20.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US$4,000.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US$4.50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US$2,250.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US$50.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US$25,000.00</t>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>WebData@123</t>
+  </si>
+  <si>
+    <t>Web Data 41</t>
+  </si>
+  <si>
+    <t>Test RateCard</t>
+  </si>
+  <si>
+    <t>rate</t>
+  </si>
+  <si>
+    <t>Test Pricing</t>
+  </si>
+  <si>
+    <t>RATE_CARD</t>
+  </si>
+  <si>
+    <t>match_column</t>
+  </si>
+  <si>
+    <t>dst</t>
+  </si>
+  <si>
+    <t>rate_test_ratecard</t>
+  </si>
+  <si>
+    <t>/test_rate_card.csv</t>
+  </si>
+  <si>
+    <t>Plan RateCard</t>
+  </si>
+  <si>
+    <t>Plan Pricing</t>
+  </si>
+  <si>
+    <t>rate_plan_ratecard</t>
+  </si>
+  <si>
+    <t>/plan_rate_card.csv</t>
+  </si>
+  <si>
+    <t>Test Category</t>
+  </si>
+  <si>
+    <t>Test Product</t>
+  </si>
+  <si>
+    <t>United States Dollar</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Items</t>
+  </si>
+  <si>
+    <t>Plan Pricing Category</t>
+  </si>
+  <si>
+    <t>Plan Pricing Product</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Plan</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>Test Customer1</t>
+  </si>
+  <si>
+    <t>Test Customer2</t>
+  </si>
+  <si>
+    <t>Test Customer3</t>
+  </si>
+  <si>
+    <t>Test Mediation</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>com.sapienter.jbilling.server.mediation.task.SeparatorFileReader</t>
+  </si>
+  <si>
+    <t>asterisk</t>
+  </si>
+  <si>
+    <t>csv</t>
+  </si>
+  <si>
+    <t>yyyyMMdd-HHmmss</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>in.webdataconsulting.jbilling.server.mediation.tasks.WebDataTestAsteriskMediationTask</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>pre paid</t>
+  </si>
+  <si>
+    <t>US$4,950.00</t>
+  </si>
+  <si>
+    <t>US$37,650.00</t>
+  </si>
+  <si>
+    <t>/MediationPlanPricing.csv</t>
+  </si>
+  <si>
+    <t>200.00</t>
+  </si>
+  <si>
+    <t>3.50</t>
+  </si>
+  <si>
+    <t>US$700.00</t>
+  </si>
+  <si>
+    <t>300.00</t>
+  </si>
+  <si>
+    <t>0.50</t>
+  </si>
+  <si>
+    <t>US$150.00</t>
+  </si>
+  <si>
+    <t>/MediationTestPricing.csv</t>
+  </si>
+  <si>
+    <t>500.00</t>
+  </si>
+  <si>
+    <t>50.00</t>
+  </si>
+  <si>
+    <t>US$25,000.00</t>
+  </si>
+  <si>
+    <t>4.50</t>
+  </si>
+  <si>
+    <t>US$2,250.00</t>
+  </si>
+  <si>
+    <t>5.00</t>
+  </si>
+  <si>
+    <t>US$2,500.00</t>
+  </si>
+  <si>
+    <t>400.00</t>
+  </si>
+  <si>
+    <t>1.50</t>
+  </si>
+  <si>
+    <t>US$600.00</t>
+  </si>
+  <si>
+    <t>15.00</t>
+  </si>
+  <si>
+    <t>US$6,000.00</t>
+  </si>
+  <si>
+    <t>2.50</t>
+  </si>
+  <si>
+    <t>US$1,250.00</t>
+  </si>
+  <si>
+    <t>20.00</t>
+  </si>
+  <si>
+    <t>US$4,000.00</t>
   </si>
 </sst>
 </file>
@@ -223,7 +218,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="5">
@@ -340,19 +335,19 @@
   </sheetPr>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="16.07"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.3148148148148"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.8074074074074"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.0148148148148"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="16.0703703703704"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -410,7 +405,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -425,23 +420,23 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="1" sqref="C1 J1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="3.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="6.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1019" min="9" style="1" width="14.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1020" style="0" width="8.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="8.36"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.2888888888889"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.1481481481481"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.2148148148148"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.2592592592593"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.3"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.8"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="3.52962962962963"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="6.17407407407407"/>
+    <col collapsed="false" hidden="false" max="1019" min="9" style="1" width="14.9"/>
+    <col collapsed="false" hidden="false" max="1023" min="1020" style="0" width="8.48518518518519"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.36296296296296"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -493,7 +488,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -508,25 +503,25 @@
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="1" sqref="C1 F8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="32.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="21.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="33.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="24.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="22.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="28.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="1" width="14.9"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.3592592592593"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.8111111111111"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.4555555555556"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.8"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.8074074074074"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="32.5259259259259"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="21.1740740740741"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="33.1074074074074"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="24.7"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="22.7296296296296"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="28.9074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="14.9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -571,7 +566,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -586,24 +581,24 @@
   </sheetPr>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="1" sqref="C1 H1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="84.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="9.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="19.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="5.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="11" style="1" width="9.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1023" style="0" width="9.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="8.36"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.662962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.00740740740741"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.5111111111111"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.00740740740741"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="84.0185185185185"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="9.00740740740741"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.3"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="5.18888888888889"/>
+    <col collapsed="false" hidden="false" max="1022" min="11" style="1" width="9.00740740740741"/>
+    <col collapsed="false" hidden="false" max="1023" min="1023" style="0" width="9.00740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.36296296296296"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -652,7 +647,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -667,27 +662,27 @@
   </sheetPr>
   <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="9.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="9.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="15.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="9.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="14.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="1" width="9.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="22.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="1" width="9.01"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="9.00740740740741"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.9407407407407"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.9925925925926"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="9.00740740740741"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.1074074074074"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.2296296296296"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="1" width="9.00740740740741"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="14.2074074074074"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="14.7"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="1" width="9.00740740740741"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="14.1111111111111"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="22.2888888888889"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="1" width="9.00740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -751,44 +746,44 @@
         <v>43</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="K3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="M3" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="O3" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="P3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K4" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K4" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>51</v>
@@ -797,7 +792,7 @@
         <v>52</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="P4" s="3" t="s">
         <v>53</v>
@@ -806,7 +801,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K5" s="3" t="s">
         <v>55</v>
       </c>
@@ -826,9 +821,9 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K6" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L6" s="3" t="s">
         <v>60</v>
@@ -837,7 +832,7 @@
         <v>61</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="P6" s="3" t="s">
         <v>62</v>
@@ -862,7 +857,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Specific Pricing Code Chnages from assert to verify in the
</commit_message>
<xml_diff>
--- a/SpecificPricing_TestData.xlsx
+++ b/SpecificPricing_TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="RateCard &amp; Pricing" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,202 +15,207 @@
     <sheet name="Orders" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="64">
   <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>WebData@123</t>
-  </si>
-  <si>
-    <t>Web Data 41</t>
-  </si>
-  <si>
-    <t>Test RateCard</t>
-  </si>
-  <si>
-    <t>rate</t>
-  </si>
-  <si>
-    <t>Test Pricing</t>
-  </si>
-  <si>
-    <t>RATE_CARD</t>
-  </si>
-  <si>
-    <t>match_column</t>
-  </si>
-  <si>
-    <t>dst</t>
-  </si>
-  <si>
-    <t>rate_test_ratecard</t>
-  </si>
-  <si>
-    <t>/test_rate_card.csv</t>
-  </si>
-  <si>
-    <t>Plan RateCard</t>
-  </si>
-  <si>
-    <t>Plan Pricing</t>
-  </si>
-  <si>
-    <t>rate_plan_ratecard</t>
-  </si>
-  <si>
-    <t>/plan_rate_card.csv</t>
-  </si>
-  <si>
-    <t>Test Category</t>
-  </si>
-  <si>
-    <t>Test Product</t>
-  </si>
-  <si>
-    <t>United States Dollar</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>Items</t>
-  </si>
-  <si>
-    <t>Plan Pricing Category</t>
-  </si>
-  <si>
-    <t>Plan Pricing Product</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>Plan</t>
-  </si>
-  <si>
-    <t>Default</t>
-  </si>
-  <si>
-    <t>Test Customer1</t>
-  </si>
-  <si>
-    <t>Test Customer2</t>
-  </si>
-  <si>
-    <t>Test Customer3</t>
-  </si>
-  <si>
-    <t>Test Mediation</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>com.sapienter.jbilling.server.mediation.task.SeparatorFileReader</t>
-  </si>
-  <si>
-    <t>asterisk</t>
-  </si>
-  <si>
-    <t>csv</t>
-  </si>
-  <si>
-    <t>yyyyMMdd-HHmmss</t>
-  </si>
-  <si>
-    <t>,</t>
-  </si>
-  <si>
-    <t>in.webdataconsulting.jbilling.server.mediation.tasks.WebDataTestAsteriskMediationTask</t>
-  </si>
-  <si>
-    <t>Monthly</t>
-  </si>
-  <si>
-    <t>pre paid</t>
-  </si>
-  <si>
-    <t>US$4,950.00</t>
-  </si>
-  <si>
-    <t>US$37,650.00</t>
-  </si>
-  <si>
-    <t>/MediationPlanPricing.csv</t>
-  </si>
-  <si>
-    <t>200.00</t>
-  </si>
-  <si>
-    <t>3.50</t>
-  </si>
-  <si>
-    <t>US$700.00</t>
-  </si>
-  <si>
-    <t>300.00</t>
-  </si>
-  <si>
-    <t>0.50</t>
-  </si>
-  <si>
-    <t>US$150.00</t>
-  </si>
-  <si>
-    <t>/MediationTestPricing.csv</t>
-  </si>
-  <si>
-    <t>500.00</t>
-  </si>
-  <si>
-    <t>50.00</t>
-  </si>
-  <si>
-    <t>US$25,000.00</t>
-  </si>
-  <si>
-    <t>4.50</t>
-  </si>
-  <si>
-    <t>US$2,250.00</t>
-  </si>
-  <si>
-    <t>5.00</t>
-  </si>
-  <si>
-    <t>US$2,500.00</t>
-  </si>
-  <si>
-    <t>400.00</t>
-  </si>
-  <si>
-    <t>1.50</t>
-  </si>
-  <si>
-    <t>US$600.00</t>
-  </si>
-  <si>
-    <t>15.00</t>
-  </si>
-  <si>
-    <t>US$6,000.00</t>
-  </si>
-  <si>
-    <t>2.50</t>
-  </si>
-  <si>
-    <t>US$1,250.00</t>
-  </si>
-  <si>
-    <t>20.00</t>
-  </si>
-  <si>
-    <t>US$4,000.00</t>
+    <t xml:space="preserve">admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WebData@123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web Data 42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test RateCard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Pricing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RATE_CARD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">match_column</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rate_test_ratecard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/test_rate_card.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan RateCard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Pricing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rate_plan_ratecard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/plan_rate_card.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United States Dollar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Pricing Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Pricing Product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Customer1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Customer2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Customer3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Mediation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.sapienter.jbilling.server.mediation.task.SeparatorFileReader</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asterisk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yyyyMMdd-HHmmss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in.webdataconsulting.jbilling.server.mediation.tasks.WebDataTestAsteriskMediationTask</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monthly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pre paid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$4,950.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$37,650.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/MediationPlanPricing.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">500.0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.5000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2250.0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50.0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25000.0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/MediationTestPricing.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200.0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.5000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">700.0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4000.0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.5000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1250.0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2500.0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">400.0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">600.0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15.0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6000.0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">300.0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150.0000</t>
   </si>
 </sst>
 </file>
@@ -218,7 +223,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="5">
@@ -335,19 +340,19 @@
   </sheetPr>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.3148148148148"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.8074074074074"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="16.0703703703704"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="16.07"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -405,7 +410,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -420,23 +425,23 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.2888888888889"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.1481481481481"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.2148148148148"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.2592592592593"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.3"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.8"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="3.52962962962963"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="6.17407407407407"/>
-    <col collapsed="false" hidden="false" max="1019" min="9" style="1" width="14.9"/>
-    <col collapsed="false" hidden="false" max="1023" min="1020" style="0" width="8.48518518518519"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.36296296296296"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="3.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="6.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1019" min="9" style="1" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1020" style="0" width="8.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="8.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -488,7 +493,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -503,25 +508,25 @@
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.3592592592593"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.8111111111111"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.4555555555556"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.8"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.8074074074074"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="32.5259259259259"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="21.1740740740741"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="33.1074074074074"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="24.7"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="22.7296296296296"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="28.9074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="1" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="32.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="21.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="33.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="24.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="22.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="28.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="1" width="14.9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -566,7 +571,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -581,24 +586,24 @@
   </sheetPr>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.662962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.00740740740741"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.5111111111111"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.00740740740741"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="84.0185185185185"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="9.00740740740741"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.3"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="5.18888888888889"/>
-    <col collapsed="false" hidden="false" max="1022" min="11" style="1" width="9.00740740740741"/>
-    <col collapsed="false" hidden="false" max="1023" min="1023" style="0" width="9.00740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.36296296296296"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="84.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="9.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="19.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="5.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="11" style="1" width="9.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1023" style="0" width="9.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="8.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -647,7 +652,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -660,32 +665,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R10"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="9.00740740740741"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.9407407407407"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.9925925925926"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="9.00740740740741"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.1074074074074"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.2296296296296"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="1" width="9.00740740740741"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="14.2074074074074"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="14.7"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="1" width="9.00740740740741"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="14.1111111111111"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="22.2888888888889"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="1" width="9.00740740740741"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="9.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="9.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="9.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="1" width="9.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="22.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="1" width="9.01"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -746,16 +751,16 @@
         <v>43</v>
       </c>
       <c r="O2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -763,101 +768,91 @@
         <v>27</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>51</v>
+        <v>41</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>53</v>
+        <v>41</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K5" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O5" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="M5" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="P5" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K6" s="3" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="M6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="O6" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="P6" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="Q6" s="3" t="s">
+      <c r="Q6" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" display="WebData@123"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>

</xml_diff>